<commit_message>
Move staff codes into questionnaire annex.
</commit_message>
<xml_diff>
--- a/Questionnaire/QuestionnaireAnnexes.xlsx
+++ b/Questionnaire/QuestionnaireAnnexes.xlsx
@@ -1,31 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh\Documents\cspro\Workshops\CSProMobileWorkshop\Questionnaire\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\work\github\CSProMobileWorkshop\Questionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C3458C3C-BADC-4571-A96E-31DA5FE1F627}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34440" windowHeight="7896" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34440" windowHeight="7896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ANN 1- Province Codes" sheetId="3" r:id="rId1"/>
-    <sheet name="ANN 2-District Codes" sheetId="12" r:id="rId2"/>
-    <sheet name="ANN 3-Birthplace Codes" sheetId="14" r:id="rId3"/>
-    <sheet name="ANN 4- Possession Value Limits" sheetId="15" r:id="rId4"/>
+    <sheet name="ANN 1 - Province Codes" sheetId="3" r:id="rId1"/>
+    <sheet name="ANN 2 - District Codes" sheetId="12" r:id="rId2"/>
+    <sheet name="ANN 3 - Birthplace Codes" sheetId="14" r:id="rId3"/>
+    <sheet name="ANN 4 - Possession Value Limits" sheetId="15" r:id="rId4"/>
+    <sheet name="ANN 5 - Staff Codes" sheetId="16" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="2">'ANN 3-Birthplace Codes'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'ANN 3 - Birthplace Codes'!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="299">
   <si>
     <t>Name</t>
   </si>
@@ -892,12 +894,45 @@
   </si>
   <si>
     <t>Place</t>
+  </si>
+  <si>
+    <t>Staff code</t>
+  </si>
+  <si>
+    <t>Role (1=interviewer, 2=supervisor)</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>EA</t>
+  </si>
+  <si>
+    <t>Shemika Rothenberger  </t>
+  </si>
+  <si>
+    <t>Andrew Benninger  </t>
+  </si>
+  <si>
+    <t>Angelica Swenson  </t>
+  </si>
+  <si>
+    <t>Zelma Hawke  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Willis Catron </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="000"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -939,7 +974,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -952,8 +987,14 @@
         <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1050,13 +1091,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1081,35 +1137,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="22">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
@@ -1355,11 +1394,33 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="wholeTable" dxfId="21"/>
+      <tableStyleElement type="headerRow" dxfId="20"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1374,52 +1435,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B8" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19">
-  <autoFilter ref="A1:B8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:B8" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17">
+  <autoFilter ref="A1:B8" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="2">
-    <tableColumn id="2" name="Name" dataDxfId="18"/>
-    <tableColumn id="3" name="Code" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Code" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D61" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13">
-  <autoFilter ref="A1:D61"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:D61" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11">
+  <autoFilter ref="A1:D61" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="5" name="Province Name" dataDxfId="12"/>
-    <tableColumn id="1" name="Province Code" dataDxfId="11"/>
-    <tableColumn id="6" name="District Name" dataDxfId="10"/>
-    <tableColumn id="3" name="District Code" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Province Name" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Province Code" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="District Name" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="District Code" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:C255" totalsRowShown="0" dataDxfId="8">
-  <autoFilter ref="A1:C255"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table5" displayName="Table5" ref="A1:C255" totalsRowShown="0" dataDxfId="6">
+  <autoFilter ref="A1:C255" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <sortState ref="A4:C197">
     <sortCondition ref="C3:C197"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="2" name="Continent" dataDxfId="7"/>
-    <tableColumn id="3" name="Place" dataDxfId="6"/>
-    <tableColumn id="4" name="Code" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Continent" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Place" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Code" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A3:D13" totalsRowShown="0">
-  <autoFilter ref="A3:D13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table4" displayName="Table4" ref="A3:D13" totalsRowShown="0">
+  <autoFilter ref="A3:D13" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Code"/>
-    <tableColumn id="2" name="Description" dataDxfId="4"/>
-    <tableColumn id="3" name="Minimum value" dataDxfId="3"/>
-    <tableColumn id="4" name="Maximum Value" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Code"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Description" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Minimum value" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Maximum Value" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1745,10 +1806,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -1835,7 +1896,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2720,7 +2781,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C255"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
@@ -5432,10 +5493,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -5614,4 +5675,146 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F1B017-425D-4710-BC42-506A76231C28}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="8" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.77734375" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="25">
+        <v>1</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2" s="26">
+        <v>2</v>
+      </c>
+      <c r="D2" s="26">
+        <v>1</v>
+      </c>
+      <c r="E2" s="26">
+        <v>1</v>
+      </c>
+      <c r="F2" s="26"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="25">
+        <v>2</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" s="26">
+        <v>1</v>
+      </c>
+      <c r="D3" s="26">
+        <v>1</v>
+      </c>
+      <c r="E3" s="26">
+        <v>1</v>
+      </c>
+      <c r="F3" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="25">
+        <v>3</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>296</v>
+      </c>
+      <c r="C4" s="26">
+        <v>1</v>
+      </c>
+      <c r="D4" s="26">
+        <v>1</v>
+      </c>
+      <c r="E4" s="26">
+        <v>1</v>
+      </c>
+      <c r="F4" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="25">
+        <v>4</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>297</v>
+      </c>
+      <c r="C5" s="26">
+        <v>1</v>
+      </c>
+      <c r="D5" s="26">
+        <v>1</v>
+      </c>
+      <c r="E5" s="26">
+        <v>1</v>
+      </c>
+      <c r="F5" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="25">
+        <v>5</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="C6" s="26">
+        <v>1</v>
+      </c>
+      <c r="D6" s="26">
+        <v>1</v>
+      </c>
+      <c r="E6" s="26">
+        <v>1</v>
+      </c>
+      <c r="F6" s="26">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>